<commit_message>
add validation job for product bulk upload
</commit_message>
<xml_diff>
--- a/public/reports/validation_report.xlsx
+++ b/public/reports/validation_report.xlsx
@@ -15,21 +15,459 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="151">
   <si>
     <t>Error Message</t>
   </si>
   <si>
-    <t>Cell B4: The Product Name field is required.</t>
-  </si>
-  <si>
-    <t>Cell D4: The Unit of Sale field is required.</t>
-  </si>
-  <si>
-    <t>Cell F4: The Manufacturer field is required.</t>
-  </si>
-  <si>
-    <t>Cell G4: The Tags field is required.</t>
+    <t>Cell AY4: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell AZ4: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell BA4: The Unit Price field is required.</t>
+  </si>
+  <si>
+    <t>Cell BY4: The Sample Available field is required.</t>
+  </si>
+  <si>
+    <t>Cell CB4: The Length field is required.</t>
+  </si>
+  <si>
+    <t>Cell CC4: The Width field is required.</t>
+  </si>
+  <si>
+    <t>Cell CD4: The Height field is required.</t>
+  </si>
+  <si>
+    <t>Cell CE4: The Weight field is required.</t>
+  </si>
+  <si>
+    <t>Cell CF4: The Breakable field is required.</t>
+  </si>
+  <si>
+    <t>Cell CG4: The Min. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CH4: The Max. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CJ4: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CK4: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CL4: The Shipper field is required.</t>
+  </si>
+  <si>
+    <t>Cell CM4: The Order Preparation Days field is required.</t>
+  </si>
+  <si>
+    <t>Cell AY5: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell AZ5: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell BA5: The Unit Price field is required.</t>
+  </si>
+  <si>
+    <t>Cell BY5: The Sample Available field is required.</t>
+  </si>
+  <si>
+    <t>Cell CB5: The Length field is required.</t>
+  </si>
+  <si>
+    <t>Cell CC5: The Width field is required.</t>
+  </si>
+  <si>
+    <t>Cell CD5: The Height field is required.</t>
+  </si>
+  <si>
+    <t>Cell CE5: The Weight field is required.</t>
+  </si>
+  <si>
+    <t>Cell CF5: The Breakable field is required.</t>
+  </si>
+  <si>
+    <t>Cell CG5: The Min. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CH5: The Max. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CJ5: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CK5: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CL5: The Shipper field is required.</t>
+  </si>
+  <si>
+    <t>Cell CM5: The Order Preparation Days field is required.</t>
+  </si>
+  <si>
+    <t>Cell AY6: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell AZ6: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell BA6: The Unit Price field is required.</t>
+  </si>
+  <si>
+    <t>Cell BY6: The Sample Available field is required.</t>
+  </si>
+  <si>
+    <t>Cell CB6: The Length field is required.</t>
+  </si>
+  <si>
+    <t>Cell CC6: The Width field is required.</t>
+  </si>
+  <si>
+    <t>Cell CD6: The Height field is required.</t>
+  </si>
+  <si>
+    <t>Cell CE6: The Weight field is required.</t>
+  </si>
+  <si>
+    <t>Cell CF6: The Breakable field is required.</t>
+  </si>
+  <si>
+    <t>Cell CG6: The Min. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CH6: The Max. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CJ6: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CK6: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CL6: The Shipper field is required.</t>
+  </si>
+  <si>
+    <t>Cell CM6: The Order Preparation Days field is required.</t>
+  </si>
+  <si>
+    <t>Cell AY7: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell AZ7: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell BA7: The Unit Price field is required.</t>
+  </si>
+  <si>
+    <t>Cell BY7: The Sample Available field is required.</t>
+  </si>
+  <si>
+    <t>Cell CB7: The Length field is required.</t>
+  </si>
+  <si>
+    <t>Cell CC7: The Width field is required.</t>
+  </si>
+  <si>
+    <t>Cell CD7: The Height field is required.</t>
+  </si>
+  <si>
+    <t>Cell CE7: The Weight field is required.</t>
+  </si>
+  <si>
+    <t>Cell CF7: The Breakable field is required.</t>
+  </si>
+  <si>
+    <t>Cell CG7: The Min. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CH7: The Max. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CJ7: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CK7: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CL7: The Shipper field is required.</t>
+  </si>
+  <si>
+    <t>Cell CM7: The Order Preparation Days field is required.</t>
+  </si>
+  <si>
+    <t>Cell AY8: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell AZ8: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell BA8: The Unit Price field is required.</t>
+  </si>
+  <si>
+    <t>Cell BY8: The Sample Available field is required.</t>
+  </si>
+  <si>
+    <t>Cell CB8: The Length field is required.</t>
+  </si>
+  <si>
+    <t>Cell CC8: The Width field is required.</t>
+  </si>
+  <si>
+    <t>Cell CD8: The Height field is required.</t>
+  </si>
+  <si>
+    <t>Cell CE8: The Weight field is required.</t>
+  </si>
+  <si>
+    <t>Cell CF8: The Breakable field is required.</t>
+  </si>
+  <si>
+    <t>Cell CG8: The Min. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CH8: The Max. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CJ8: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CK8: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CL8: The Shipper field is required.</t>
+  </si>
+  <si>
+    <t>Cell CM8: The Order Preparation Days field is required.</t>
+  </si>
+  <si>
+    <t>Cell AY9: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell AZ9: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell BA9: The Unit Price field is required.</t>
+  </si>
+  <si>
+    <t>Cell BY9: The Sample Available field is required.</t>
+  </si>
+  <si>
+    <t>Cell CB9: The Length field is required.</t>
+  </si>
+  <si>
+    <t>Cell CC9: The Width field is required.</t>
+  </si>
+  <si>
+    <t>Cell CD9: The Height field is required.</t>
+  </si>
+  <si>
+    <t>Cell CE9: The Weight field is required.</t>
+  </si>
+  <si>
+    <t>Cell CF9: The Breakable field is required.</t>
+  </si>
+  <si>
+    <t>Cell CG9: The Min. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CH9: The Max. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CJ9: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CK9: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CL9: The Shipper field is required.</t>
+  </si>
+  <si>
+    <t>Cell CM9: The Order Preparation Days field is required.</t>
+  </si>
+  <si>
+    <t>Cell AY10: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell AZ10: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell BA10: The Unit Price field is required.</t>
+  </si>
+  <si>
+    <t>Cell BY10: The Sample Available field is required.</t>
+  </si>
+  <si>
+    <t>Cell CB10: The Length field is required.</t>
+  </si>
+  <si>
+    <t>Cell CC10: The Width field is required.</t>
+  </si>
+  <si>
+    <t>Cell CD10: The Height field is required.</t>
+  </si>
+  <si>
+    <t>Cell CE10: The Weight field is required.</t>
+  </si>
+  <si>
+    <t>Cell CF10: The Breakable field is required.</t>
+  </si>
+  <si>
+    <t>Cell CG10: The Min. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CH10: The Max. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CJ10: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CK10: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CL10: The Shipper field is required.</t>
+  </si>
+  <si>
+    <t>Cell CM10: The Order Preparation Days field is required.</t>
+  </si>
+  <si>
+    <t>Cell AY11: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell AZ11: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell BA11: The Unit Price field is required.</t>
+  </si>
+  <si>
+    <t>Cell BY11: The Sample Available field is required.</t>
+  </si>
+  <si>
+    <t>Cell CB11: The Length field is required.</t>
+  </si>
+  <si>
+    <t>Cell CC11: The Width field is required.</t>
+  </si>
+  <si>
+    <t>Cell CD11: The Height field is required.</t>
+  </si>
+  <si>
+    <t>Cell CE11: The Weight field is required.</t>
+  </si>
+  <si>
+    <t>Cell CF11: The Breakable field is required.</t>
+  </si>
+  <si>
+    <t>Cell CG11: The Min. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CH11: The Max. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CJ11: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CK11: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CL11: The Shipper field is required.</t>
+  </si>
+  <si>
+    <t>Cell CM11: The Order Preparation Days field is required.</t>
+  </si>
+  <si>
+    <t>Cell AY12: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell AZ12: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell BA12: The Unit Price field is required.</t>
+  </si>
+  <si>
+    <t>Cell BY12: The Sample Available field is required.</t>
+  </si>
+  <si>
+    <t>Cell CB12: The Length field is required.</t>
+  </si>
+  <si>
+    <t>Cell CC12: The Width field is required.</t>
+  </si>
+  <si>
+    <t>Cell CD12: The Height field is required.</t>
+  </si>
+  <si>
+    <t>Cell CE12: The Weight field is required.</t>
+  </si>
+  <si>
+    <t>Cell CF12: The Breakable field is required.</t>
+  </si>
+  <si>
+    <t>Cell CG12: The Min. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CH12: The Max. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CJ12: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CK12: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CL12: The Shipper field is required.</t>
+  </si>
+  <si>
+    <t>Cell CM12: The Order Preparation Days field is required.</t>
+  </si>
+  <si>
+    <t>Cell AY13: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell AZ13: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell BA13: The Unit Price field is required.</t>
+  </si>
+  <si>
+    <t>Cell BY13: The Sample Available field is required.</t>
+  </si>
+  <si>
+    <t>Cell CB13: The Length field is required.</t>
+  </si>
+  <si>
+    <t>Cell CC13: The Width field is required.</t>
+  </si>
+  <si>
+    <t>Cell CD13: The Height field is required.</t>
+  </si>
+  <si>
+    <t>Cell CE13: The Weight field is required.</t>
+  </si>
+  <si>
+    <t>Cell CF13: The Breakable field is required.</t>
+  </si>
+  <si>
+    <t>Cell CG13: The Min. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CH13: The Max. Temperature field is required.</t>
+  </si>
+  <si>
+    <t>Cell CJ13: The From Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CK13: The To Quantity field is required.</t>
+  </si>
+  <si>
+    <t>Cell CL13: The Shipper field is required.</t>
+  </si>
+  <si>
+    <t>Cell CM13: The Order Preparation Days field is required.</t>
   </si>
 </sst>
 </file>
@@ -369,7 +807,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -400,6 +838,736 @@
     <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>